<commit_message>
Mccalluc/more field templates (#722)
* library_id: Not sure if longer description holds for all

* library_layout

* library_final_yield

* library_concentration_value_unit

* regen
</commit_message>
<xml_diff>
--- a/docs/bulkatacseq/bulkatacseq-metadata.xlsx
+++ b/docs/bulkatacseq/bulkatacseq-metadata.xlsx
@@ -360,7 +360,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Total amount (eg. nanograms) of library after the clean-up step of final pcr amplification step. Answer the question: What is the Qubit measured concentration (ng/ul) times the elution volume (ul) after the final clean-up step?</t>
+          <t>Total number of ng of library after final pcr amplification step. This is the concentration (ng/ul) * volume (ul)</t>
         </r>
       </text>
     </comment>
@@ -373,7 +373,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Units of library final yield</t>
+          <t>Units of final library yield</t>
         </r>
       </text>
     </comment>
@@ -386,7 +386,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ID of the library sample.</t>
+          <t>A library ID, unique within a TMC, which allows corresponding RNA and chromatin accessibility datasets to be linked.</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Tweak schemas to get consistent field types
</commit_message>
<xml_diff>
--- a/docs/bulkatacseq/bulkatacseq-metadata.xlsx
+++ b/docs/bulkatacseq/bulkatacseq-metadata.xlsx
@@ -295,7 +295,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Average size in basepairs (bp) of sequencing library fragments estimated via gel electrophoresis or Bioanalyzer/tapestation.</t>
+          <t>Average size in basepairs (bp) of sequencing library fragments estimated via gel electrophoresis or bioanalyzer/tapestation.</t>
         </r>
       </text>
     </comment>
@@ -1194,7 +1194,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="14">
+  <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1212,6 +1212,10 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="S2:S1048576">
       <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="U2:U1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="V2:V1048576">
       <formula1>-1e+307</formula1>

</xml_diff>